<commit_message>
fix urban_ath 1_1 urb_area_id 1804 Rennes
</commit_message>
<xml_diff>
--- a/dictionaries/urban_ath/1_1/1_1_non_rep.xlsx
+++ b/dictionaries/urban_ath/1_1/1_1_non_rep.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26704"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PROJECTS\ATHLETE\DOCUMENTS\dictionaries\jose_dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="13_ncr:1_{3C7DCB47-9CAD-40CA-9189-C25A657794B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DEC48EA2-659A-4168-9B93-51CACEBF0475}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:1_{3C7DCB47-9CAD-40CA-9189-C25A657794B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11329D87-91D6-4D07-8817-355DA2679FFC}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,9 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -1872,7 +1875,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1900,7 +1903,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="41">
     <cellStyle name="20% - Accent1" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -2325,7 +2327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMH176"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
@@ -4450,7 +4452,7 @@
       <c r="B80" t="s">
         <v>18</v>
       </c>
-      <c r="C80" s="17" t="s">
+      <c r="C80" t="s">
         <v>181</v>
       </c>
       <c r="D80" t="s">
@@ -4478,7 +4480,7 @@
       <c r="B82" t="s">
         <v>18</v>
       </c>
-      <c r="C82" s="17" t="s">
+      <c r="C82" t="s">
         <v>186</v>
       </c>
       <c r="D82" t="s">
@@ -5785,8 +5787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E173"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D33"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75"/>
@@ -6669,7 +6671,7 @@
         <v>233</v>
       </c>
       <c r="B63">
-        <v>1803</v>
+        <v>1804</v>
       </c>
       <c r="C63" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
convert valueType binary to boolean
</commit_message>
<xml_diff>
--- a/dictionaries/urban_ath/1_1/1_1_non_rep.xlsx
+++ b/dictionaries/urban_ath/1_1/1_1_non_rep.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PROJECTS\ATHLETE\DOCUMENTS\dictionaries\jose_dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:1_{3C7DCB47-9CAD-40CA-9189-C25A657794B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11329D87-91D6-4D07-8817-355DA2679FFC}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="13_ncr:1_{3C7DCB47-9CAD-40CA-9189-C25A657794B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EB7DCC2-E599-4BC9-AF49-3FD3C8BBAEB5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -159,7 +159,7 @@
     <t>ath_blueyn300_preg</t>
   </si>
   <si>
-    <t>binary</t>
+    <t>boolean</t>
   </si>
   <si>
     <t>is there a blue space  &gt; 5,000 m2 in a distance of 300 m? at pregnancy</t>
@@ -2327,8 +2327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMH176"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75"/>
@@ -5787,7 +5787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>

</xml_diff>